<commit_message>
Functionality testing Scripts for issue #1 and #2 in proj:App2Automate -
</commit_message>
<xml_diff>
--- a/WebAppAutomation/Files/ExcelFiles/TestData_WebApp.xlsx
+++ b/WebAppAutomation/Files/ExcelFiles/TestData_WebApp.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="23">
   <si>
     <t>Email_TestData</t>
   </si>
@@ -24,25 +24,70 @@
     <t>Email_TestData_Result</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
     <t>test@test.com</t>
   </si>
   <si>
-    <t>test.com</t>
-  </si>
-  <si>
-    <t>test###</t>
-  </si>
-  <si>
     <t>test@.com</t>
   </si>
   <si>
-    <t>###@t.com</t>
-  </si>
-  <si>
-    <t>Pass</t>
+    <t>UserName_TestData</t>
+  </si>
+  <si>
+    <t>UserName_TestData_Result</t>
+  </si>
+  <si>
+    <t>Test_Data_Type</t>
+  </si>
+  <si>
+    <t>Both Positive</t>
+  </si>
+  <si>
+    <t>UN positive
+Email Negative</t>
+  </si>
+  <si>
+    <t>Both blank values</t>
+  </si>
+  <si>
+    <t>UN blank
+Email positive</t>
+  </si>
+  <si>
+    <t>UN positive
+Email Blank</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>Tester2</t>
+  </si>
+  <si>
+    <t>test2@test.com</t>
+  </si>
+  <si>
+    <t>Tester3</t>
+  </si>
+  <si>
+    <t>test@1.2</t>
+  </si>
+  <si>
+    <t>!@#$%</t>
+  </si>
+  <si>
+    <t>A@#$123;</t>
+  </si>
+  <si>
+    <t>#$@.com</t>
+  </si>
+  <si>
+    <t>Testcase Passed</t>
+  </si>
+  <si>
+    <t>Testcase Pass</t>
+  </si>
+  <si>
+    <t>Testcase Failed</t>
   </si>
 </sst>
 </file>
@@ -50,8 +95,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -79,8 +132,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,72 +432,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="24.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="37.5" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
+      <c r="B7">
         <v>123456</v>
       </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>123456</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30">
+      <c r="A8" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>